<commit_message>
Conversão CAN, ajustes em módulos
Adicionados valores no Gateway para converter os dados da rede CAN novamente para valores "certos".
</commit_message>
<xml_diff>
--- a/Firmwares/Tabela de codificação de sensores.xlsx
+++ b/Firmwares/Tabela de codificação de sensores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe-PC\Desktop\EK304\Firmwares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE0A70C-0BBC-40B5-9EA3-FB4DA9BB2C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3FBB74-31FD-4F07-AEB1-6633114EFA38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,24 +399,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Vitor Gervasi Adão:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Suspensão: O valor está limitado entre: 126 a 876, no código aplicou-se a função map() o qual torna os limites de: 0 a 90.
-Valores de 0 a 90.</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Suspensão: O valor está limitado entre: 126 a 876, no código aplicou-se a função map() o qual torna os limites de: 0 a 255.
+Valores de 0 a 255</t>
         </r>
       </text>
     </comment>
@@ -424,24 +413,13 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Vitor Gervasi Adão:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Suspensão: O valor está limitado entre: 126 a 876, no código aplicou-se a função map() o qual torna os limites de: 0 a 90.
-Valores de 0 a 90.</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Suspensão: O valor está limitado entre: 126 a 876, no código aplicou-se a função map() o qual torna os limites de: 0 a 255.
+Valores de 0 a 255.</t>
         </r>
       </text>
     </comment>
@@ -1378,10 +1356,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -1425,7 +1399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1477,7 +1451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1681,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Criação do arquivo DBC
Início da adaptação da programação da CAN de modo que seja escalável.
</commit_message>
<xml_diff>
--- a/Firmwares/Tabela de codificação de sensores.xlsx
+++ b/Firmwares/Tabela de codificação de sensores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe-PC\Desktop\EK304\Firmwares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3FBB74-31FD-4F07-AEB1-6633114EFA38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2750E53C-503F-462E-B5BD-5C8219CC8252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,58 +576,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="J26" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Digitos mais significativos</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K26" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Digitos menos significativos</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L26" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Digitos mais significativos</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M26" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Digitos menos significativos</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="I33" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
@@ -776,7 +724,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="113">
   <si>
     <t>0x00</t>
   </si>
@@ -1024,6 +972,123 @@
   <si>
     <t>3</t>
   </si>
+  <si>
+    <t>LENGTH</t>
+  </si>
+  <si>
+    <t>MODULE</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>Gyro01</t>
+  </si>
+  <si>
+    <t>Acc01</t>
+  </si>
+  <si>
+    <t>Acc03</t>
+  </si>
+  <si>
+    <t>Acc02</t>
+  </si>
+  <si>
+    <t>Gyro02</t>
+  </si>
+  <si>
+    <t>Gyro03</t>
+  </si>
+  <si>
+    <t>GearPosition</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>OilPressure</t>
+  </si>
+  <si>
+    <t>OilTemp</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>AirTemp</t>
+  </si>
+  <si>
+    <t>WaterTemp</t>
+  </si>
+  <si>
+    <t>TPS</t>
+  </si>
+  <si>
+    <t>LambdaFactor</t>
+  </si>
+  <si>
+    <t>MAP</t>
+  </si>
+  <si>
+    <t>SuspRear</t>
+  </si>
+  <si>
+    <t>SuspFront</t>
+  </si>
 </sst>
 </file>
 
@@ -1032,7 +1097,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;0x&quot;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1080,14 +1145,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1146,7 +1203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1268,11 +1325,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1299,7 +1530,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1338,6 +1569,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1656,7 +1929,7 @@
   <dimension ref="B1:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1940,10 @@
     <col min="6" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="4.42578125" customWidth="1"/>
     <col min="17" max="17" width="29.85546875" customWidth="1"/>
-    <col min="18" max="28" width="9.140625" style="1"/>
+    <col min="18" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="22.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" style="1" customWidth="1"/>
+    <col min="22" max="28" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1692,10 +1968,18 @@
       </c>
       <c r="Q2" s="22"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
+      <c r="S2" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>75</v>
+      </c>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
@@ -1724,10 +2008,18 @@
       <c r="P3" s="23"/>
       <c r="Q3" s="24"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
+      <c r="S3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="U3" s="30">
+        <v>2</v>
+      </c>
+      <c r="V3" s="32">
+        <v>2</v>
+      </c>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -1778,10 +2070,18 @@
       <c r="P4" s="23"/>
       <c r="Q4" s="24"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
+      <c r="S4" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="U4" s="37">
+        <v>3</v>
+      </c>
+      <c r="V4" s="38">
+        <v>1</v>
+      </c>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
@@ -1825,10 +2125,18 @@
       <c r="P5" s="23"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
+      <c r="S5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="U5" s="30">
+        <v>3</v>
+      </c>
+      <c r="V5" s="32">
+        <v>1</v>
+      </c>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -1872,10 +2180,18 @@
       <c r="P6" s="23"/>
       <c r="Q6" s="24"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
+      <c r="S6" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="T6" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="U6" s="30">
+        <v>3</v>
+      </c>
+      <c r="V6" s="32">
+        <v>1</v>
+      </c>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -1919,10 +2235,18 @@
       <c r="P7" s="23"/>
       <c r="Q7" s="24"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
+      <c r="S7" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="T7" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="U7" s="30">
+        <v>3</v>
+      </c>
+      <c r="V7" s="32">
+        <v>1</v>
+      </c>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -1934,10 +2258,18 @@
       <c r="P8" s="23"/>
       <c r="Q8" s="24"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
+      <c r="S8" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="U8" s="30">
+        <v>3</v>
+      </c>
+      <c r="V8" s="32">
+        <v>4</v>
+      </c>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -1964,10 +2296,18 @@
       <c r="P9" s="23"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
+      <c r="S9" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="U9" s="30">
+        <v>3</v>
+      </c>
+      <c r="V9" s="32">
+        <v>4</v>
+      </c>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -1996,10 +2336,18 @@
       <c r="P10" s="23"/>
       <c r="Q10" s="24"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
+      <c r="S10" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="T10" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="U10" s="30">
+        <v>1</v>
+      </c>
+      <c r="V10" s="32">
+        <v>2</v>
+      </c>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -2050,10 +2398,18 @@
       <c r="P11" s="23"/>
       <c r="Q11" s="24"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
+      <c r="S11" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="T11" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="U11" s="30">
+        <v>1</v>
+      </c>
+      <c r="V11" s="32">
+        <v>3</v>
+      </c>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -2103,10 +2459,18 @@
       <c r="P12" s="23"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
+      <c r="S12" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="T12" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="U12" s="30">
+        <v>2</v>
+      </c>
+      <c r="V12" s="32">
+        <v>3</v>
+      </c>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -2156,10 +2520,18 @@
       <c r="P13" s="23"/>
       <c r="Q13" s="24"/>
       <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
+      <c r="S13" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="T13" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="U13" s="30">
+        <v>2</v>
+      </c>
+      <c r="V13" s="32">
+        <v>3</v>
+      </c>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
@@ -2201,10 +2573,18 @@
       <c r="P14" s="23"/>
       <c r="Q14" s="24"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
+      <c r="S14" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="T14" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="U14" s="30">
+        <v>3</v>
+      </c>
+      <c r="V14" s="32">
+        <v>4</v>
+      </c>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -2216,10 +2596,18 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
+      <c r="S15" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="T15" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="U15" s="30">
+        <v>1</v>
+      </c>
+      <c r="V15" s="32">
+        <v>4</v>
+      </c>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
@@ -2246,10 +2634,18 @@
       <c r="P16" s="23"/>
       <c r="Q16" s="24"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
+      <c r="S16" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="T16" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="U16" s="30">
+        <v>1</v>
+      </c>
+      <c r="V16" s="32">
+        <v>4</v>
+      </c>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -2278,10 +2674,18 @@
       <c r="P17" s="23"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
+      <c r="S17" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="T17" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="U17" s="30">
+        <v>1</v>
+      </c>
+      <c r="V17" s="32">
+        <v>4</v>
+      </c>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -2332,10 +2736,18 @@
       <c r="P18" s="23"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
+      <c r="S18" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="T18" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="U18" s="30">
+        <v>1</v>
+      </c>
+      <c r="V18" s="32">
+        <v>2</v>
+      </c>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
@@ -2385,10 +2797,18 @@
       <c r="P19" s="23"/>
       <c r="Q19" s="24"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
+      <c r="S19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="T19" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="U19" s="30">
+        <v>1</v>
+      </c>
+      <c r="V19" s="32">
+        <v>2</v>
+      </c>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
@@ -2416,10 +2836,18 @@
       <c r="P20" s="23"/>
       <c r="Q20" s="24"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
+      <c r="S20" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="T20" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="U20" s="30">
+        <v>1</v>
+      </c>
+      <c r="V20" s="32">
+        <v>2</v>
+      </c>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
@@ -2447,10 +2875,18 @@
       <c r="P21" s="23"/>
       <c r="Q21" s="24"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
+      <c r="S21" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="T21" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="U21" s="30">
+        <v>3</v>
+      </c>
+      <c r="V21" s="32">
+        <v>1</v>
+      </c>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
@@ -2461,6 +2897,18 @@
     <row r="22" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P22" s="23"/>
       <c r="Q22" s="24"/>
+      <c r="S22" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="T22" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="U22" s="34">
+        <v>1</v>
+      </c>
+      <c r="V22" s="35">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="s">
@@ -2567,14 +3015,14 @@
       <c r="I26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13" t="s">
+      <c r="K26" s="28"/>
+      <c r="L26" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="M26" s="13"/>
+      <c r="M26" s="28"/>
       <c r="N26" s="8" t="s">
         <v>0</v>
       </c>
@@ -2811,7 +3259,9 @@
       <c r="Q35" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="H5:I5"/>

</xml_diff>